<commit_message>
Added testing for CRUD operations for customer and confirmed it worked.
</commit_message>
<xml_diff>
--- a/CMPG323 EcoPower Logistics Data.xlsx
+++ b/CMPG323 EcoPower Logistics Data.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\1_3rd_year_uni\CMPG323\CMPG323_Project4\CMPG-323-Project-4-40604012\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7DE3EDCF-8D2E-428E-AB1B-4A29BC91C1AD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F2CED0B7-B789-4E01-8CEA-42B7BBD76F4A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2340" yWindow="2340" windowWidth="15375" windowHeight="7875" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="3525" yWindow="615" windowWidth="15375" windowHeight="7875" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Customers" sheetId="1" r:id="rId1"/>
@@ -732,8 +732,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:F14"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F2" sqref="F2:F7"/>
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="F2" sqref="F2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -779,6 +779,9 @@
       <c r="E2">
         <v>5723177115</v>
       </c>
+      <c r="F2" t="b">
+        <v>1</v>
+      </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3">
@@ -796,6 +799,9 @@
       <c r="E3">
         <v>9041993848</v>
       </c>
+      <c r="F3" t="b">
+        <v>1</v>
+      </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4">
@@ -813,6 +819,9 @@
       <c r="E4">
         <v>3738283528</v>
       </c>
+      <c r="F4" t="b">
+        <v>1</v>
+      </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5">
@@ -830,6 +839,9 @@
       <c r="E5">
         <v>6447102299</v>
       </c>
+      <c r="F5" t="b">
+        <v>1</v>
+      </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6">
@@ -847,6 +859,9 @@
       <c r="E6">
         <v>1878764468</v>
       </c>
+      <c r="F6" t="b">
+        <v>1</v>
+      </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7">
@@ -864,6 +879,9 @@
       <c r="E7">
         <v>9666552669</v>
       </c>
+      <c r="F7" t="b">
+        <v>1</v>
+      </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8">
@@ -881,6 +899,9 @@
       <c r="E8">
         <v>2384982848</v>
       </c>
+      <c r="F8" t="b">
+        <v>1</v>
+      </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A9">
@@ -898,6 +919,9 @@
       <c r="E9">
         <v>8945409882</v>
       </c>
+      <c r="F9" t="b">
+        <v>1</v>
+      </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A10">
@@ -915,6 +939,9 @@
       <c r="E10">
         <v>1320602595</v>
       </c>
+      <c r="F10" t="b">
+        <v>1</v>
+      </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A11">
@@ -932,6 +959,9 @@
       <c r="E11">
         <v>7968612324</v>
       </c>
+      <c r="F11" t="b">
+        <v>1</v>
+      </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A12">
@@ -949,6 +979,9 @@
       <c r="E12">
         <v>1578247192</v>
       </c>
+      <c r="F12" t="b">
+        <v>1</v>
+      </c>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A13">
@@ -966,6 +999,9 @@
       <c r="E13">
         <v>7425817353</v>
       </c>
+      <c r="F13" t="b">
+        <v>1</v>
+      </c>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A14">
@@ -982,6 +1018,9 @@
       </c>
       <c r="E14">
         <v>5815761997</v>
+      </c>
+      <c r="F14" t="b">
+        <v>1</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Made use of an argument in main to get file path and changed window visibility settings
</commit_message>
<xml_diff>
--- a/CMPG323 EcoPower Logistics Data.xlsx
+++ b/CMPG323 EcoPower Logistics Data.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\1_3rd_year_uni\CMPG323\CMPG323_Project4\CMPG-323-Project-4-40604012\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F2CED0B7-B789-4E01-8CEA-42B7BBD76F4A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B6E2E2E6-03BF-4B80-B7BC-8C414D4D6948}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3525" yWindow="615" windowWidth="15375" windowHeight="7875" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-12030" yWindow="330" windowWidth="15375" windowHeight="7875" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Customers" sheetId="1" r:id="rId1"/>
@@ -780,7 +780,7 @@
         <v>5723177115</v>
       </c>
       <c r="F2" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Began with order testing
</commit_message>
<xml_diff>
--- a/CMPG323 EcoPower Logistics Data.xlsx
+++ b/CMPG323 EcoPower Logistics Data.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\1_3rd_year_uni\CMPG323\CMPG323_Project4\CMPG-323-Project-4-40604012\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B6E2E2E6-03BF-4B80-B7BC-8C414D4D6948}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7F5CAA5E-FA91-4763-87FF-0585FFC319A7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-12030" yWindow="330" windowWidth="15375" windowHeight="7875" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -780,7 +780,7 @@
         <v>5723177115</v>
       </c>
       <c r="F2" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Redoing customer since it is not working properly
</commit_message>
<xml_diff>
--- a/CMPG323 EcoPower Logistics Data.xlsx
+++ b/CMPG323 EcoPower Logistics Data.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\1_3rd_year_uni\CMPG323\CMPG323_Project4\CMPG-323-Project-4-40604012\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7F5CAA5E-FA91-4763-87FF-0585FFC319A7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1FCD2198-26E8-4DE4-8F17-6C7E4BC74F87}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-12030" yWindow="330" windowWidth="15375" windowHeight="7875" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -732,7 +732,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:F14"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="F2" sqref="F2"/>
     </sheetView>
   </sheetViews>
@@ -780,7 +780,7 @@
         <v>5723177115</v>
       </c>
       <c r="F2" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
@@ -859,9 +859,6 @@
       <c r="E6">
         <v>1878764468</v>
       </c>
-      <c r="F6" t="b">
-        <v>1</v>
-      </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7">
@@ -879,9 +876,6 @@
       <c r="E7">
         <v>9666552669</v>
       </c>
-      <c r="F7" t="b">
-        <v>1</v>
-      </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8">
@@ -899,9 +893,6 @@
       <c r="E8">
         <v>2384982848</v>
       </c>
-      <c r="F8" t="b">
-        <v>1</v>
-      </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A9">
@@ -919,9 +910,6 @@
       <c r="E9">
         <v>8945409882</v>
       </c>
-      <c r="F9" t="b">
-        <v>1</v>
-      </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A10">
@@ -939,9 +927,6 @@
       <c r="E10">
         <v>1320602595</v>
       </c>
-      <c r="F10" t="b">
-        <v>1</v>
-      </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A11">
@@ -959,9 +944,6 @@
       <c r="E11">
         <v>7968612324</v>
       </c>
-      <c r="F11" t="b">
-        <v>1</v>
-      </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A12">
@@ -979,9 +961,6 @@
       <c r="E12">
         <v>1578247192</v>
       </c>
-      <c r="F12" t="b">
-        <v>1</v>
-      </c>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A13">
@@ -999,9 +978,6 @@
       <c r="E13">
         <v>7425817353</v>
       </c>
-      <c r="F13" t="b">
-        <v>1</v>
-      </c>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A14">
@@ -1018,9 +994,6 @@
       </c>
       <c r="E14">
         <v>5815761997</v>
-      </c>
-      <c r="F14" t="b">
-        <v>1</v>
       </c>
     </row>
   </sheetData>
@@ -1755,7 +1728,7 @@
   <dimension ref="A1:E15"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E1" sqref="E1"/>
+      <selection activeCell="E2" sqref="E2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
finished rewriting customer testing
</commit_message>
<xml_diff>
--- a/CMPG323 EcoPower Logistics Data.xlsx
+++ b/CMPG323 EcoPower Logistics Data.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\1_3rd_year_uni\CMPG323\CMPG323_Project4\CMPG-323-Project-4-40604012\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1FCD2198-26E8-4DE4-8F17-6C7E4BC74F87}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EC3EC0BD-0FC5-47E7-9112-BA48A83A79F6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-12030" yWindow="330" windowWidth="15375" windowHeight="7875" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-18180" yWindow="-525" windowWidth="15375" windowHeight="7875" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Customers" sheetId="1" r:id="rId1"/>
@@ -780,7 +780,7 @@
         <v>5723177115</v>
       </c>
       <c r="F2" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
@@ -859,6 +859,9 @@
       <c r="E6">
         <v>1878764468</v>
       </c>
+      <c r="F6" t="b">
+        <v>1</v>
+      </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7">
@@ -876,6 +879,9 @@
       <c r="E7">
         <v>9666552669</v>
       </c>
+      <c r="F7" t="b">
+        <v>1</v>
+      </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8">
@@ -893,6 +899,9 @@
       <c r="E8">
         <v>2384982848</v>
       </c>
+      <c r="F8" t="b">
+        <v>1</v>
+      </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A9">
@@ -910,6 +919,9 @@
       <c r="E9">
         <v>8945409882</v>
       </c>
+      <c r="F9" t="b">
+        <v>1</v>
+      </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A10">
@@ -927,6 +939,9 @@
       <c r="E10">
         <v>1320602595</v>
       </c>
+      <c r="F10" t="b">
+        <v>1</v>
+      </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A11">
@@ -944,6 +959,9 @@
       <c r="E11">
         <v>7968612324</v>
       </c>
+      <c r="F11" t="b">
+        <v>1</v>
+      </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A12">
@@ -961,6 +979,9 @@
       <c r="E12">
         <v>1578247192</v>
       </c>
+      <c r="F12" t="b">
+        <v>1</v>
+      </c>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A13">
@@ -978,6 +999,9 @@
       <c r="E13">
         <v>7425817353</v>
       </c>
+      <c r="F13" t="b">
+        <v>1</v>
+      </c>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A14">
@@ -994,6 +1018,9 @@
       </c>
       <c r="E14">
         <v>5815761997</v>
+      </c>
+      <c r="F14" t="b">
+        <v>1</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Finished Order testing automation
</commit_message>
<xml_diff>
--- a/CMPG323 EcoPower Logistics Data.xlsx
+++ b/CMPG323 EcoPower Logistics Data.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\1_3rd_year_uni\CMPG323\CMPG323_Project4\CMPG-323-Project-4-40604012\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EC3EC0BD-0FC5-47E7-9112-BA48A83A79F6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{97B0001F-B576-4D74-90A6-4E9D329830AD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-18180" yWindow="-525" windowWidth="15375" windowHeight="7875" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-18180" yWindow="-525" windowWidth="15375" windowHeight="7875" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Customers" sheetId="1" r:id="rId1"/>
@@ -732,8 +732,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:F14"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F2" sqref="F2"/>
+    <sheetView topLeftCell="A11" workbookViewId="0">
+      <selection activeCell="G2" sqref="G2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1754,7 +1754,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:E15"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
       <selection activeCell="E2" sqref="E2"/>
     </sheetView>
   </sheetViews>
@@ -1797,6 +1797,9 @@
       <c r="D2" t="s">
         <v>43</v>
       </c>
+      <c r="E2" t="b">
+        <v>1</v>
+      </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3">
@@ -1811,6 +1814,9 @@
       <c r="D3" t="s">
         <v>44</v>
       </c>
+      <c r="E3" t="b">
+        <v>1</v>
+      </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4">
@@ -1825,6 +1831,9 @@
       <c r="D4" t="s">
         <v>45</v>
       </c>
+      <c r="E4" t="b">
+        <v>1</v>
+      </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5">
@@ -1839,6 +1848,9 @@
       <c r="D5" t="s">
         <v>46</v>
       </c>
+      <c r="E5" t="b">
+        <v>1</v>
+      </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6">
@@ -1853,6 +1865,9 @@
       <c r="D6" t="s">
         <v>47</v>
       </c>
+      <c r="E6" t="b">
+        <v>1</v>
+      </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7">
@@ -1867,6 +1882,9 @@
       <c r="D7" t="s">
         <v>48</v>
       </c>
+      <c r="E7" t="b">
+        <v>1</v>
+      </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8">
@@ -1881,6 +1899,9 @@
       <c r="D8" t="s">
         <v>49</v>
       </c>
+      <c r="E8" t="b">
+        <v>1</v>
+      </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9">
@@ -1895,6 +1916,9 @@
       <c r="D9" t="s">
         <v>50</v>
       </c>
+      <c r="E9" t="b">
+        <v>1</v>
+      </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A10">
@@ -1909,6 +1933,9 @@
       <c r="D10" t="s">
         <v>51</v>
       </c>
+      <c r="E10" t="b">
+        <v>1</v>
+      </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A11">
@@ -1923,6 +1950,9 @@
       <c r="D11" t="s">
         <v>52</v>
       </c>
+      <c r="E11" t="b">
+        <v>1</v>
+      </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A12">
@@ -1937,6 +1967,9 @@
       <c r="D12" t="s">
         <v>53</v>
       </c>
+      <c r="E12" t="b">
+        <v>1</v>
+      </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A13">
@@ -1951,6 +1984,9 @@
       <c r="D13" t="s">
         <v>54</v>
       </c>
+      <c r="E13" t="b">
+        <v>1</v>
+      </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A14">
@@ -1965,6 +2001,9 @@
       <c r="D14" t="s">
         <v>55</v>
       </c>
+      <c r="E14" t="b">
+        <v>1</v>
+      </c>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A15">
@@ -1978,6 +2017,9 @@
       </c>
       <c r="D15" t="s">
         <v>56</v>
+      </c>
+      <c r="E15" t="b">
+        <v>1</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Finished Product Testing Sequence
</commit_message>
<xml_diff>
--- a/CMPG323 EcoPower Logistics Data.xlsx
+++ b/CMPG323 EcoPower Logistics Data.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\1_3rd_year_uni\CMPG323\CMPG323_Project4\CMPG-323-Project-4-40604012\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{97B0001F-B576-4D74-90A6-4E9D329830AD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3F87F251-6633-489A-AC09-5E2696DD8E89}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-18180" yWindow="-525" windowWidth="15375" windowHeight="7875" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-18180" yWindow="-525" windowWidth="15375" windowHeight="7875" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Customers" sheetId="1" r:id="rId1"/>
@@ -1754,7 +1754,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:E15"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
+    <sheetView topLeftCell="A10" workbookViewId="0">
       <selection activeCell="E2" sqref="E2"/>
     </sheetView>
   </sheetViews>
@@ -2031,7 +2031,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:E40"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A31" workbookViewId="0">
       <selection activeCell="E1" sqref="E1"/>
     </sheetView>
   </sheetViews>
@@ -2074,6 +2074,9 @@
       <c r="D2">
         <v>950</v>
       </c>
+      <c r="E2" t="b">
+        <v>1</v>
+      </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3">
@@ -2088,6 +2091,9 @@
       <c r="D3">
         <v>61</v>
       </c>
+      <c r="E3" t="b">
+        <v>1</v>
+      </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4">
@@ -2102,6 +2108,9 @@
       <c r="D4">
         <v>281</v>
       </c>
+      <c r="E4" t="b">
+        <v>1</v>
+      </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5">
@@ -2116,6 +2125,9 @@
       <c r="D5">
         <v>502</v>
       </c>
+      <c r="E5" t="b">
+        <v>1</v>
+      </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6">
@@ -2130,6 +2142,9 @@
       <c r="D6">
         <v>621</v>
       </c>
+      <c r="E6" t="b">
+        <v>1</v>
+      </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7">
@@ -2144,6 +2159,9 @@
       <c r="D7">
         <v>765</v>
       </c>
+      <c r="E7" t="b">
+        <v>1</v>
+      </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8">
@@ -2158,6 +2176,9 @@
       <c r="D8">
         <v>709</v>
       </c>
+      <c r="E8" t="b">
+        <v>1</v>
+      </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9">
@@ -2172,6 +2193,9 @@
       <c r="D9">
         <v>485</v>
       </c>
+      <c r="E9" t="b">
+        <v>1</v>
+      </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A10">
@@ -2186,6 +2210,9 @@
       <c r="D10">
         <v>158</v>
       </c>
+      <c r="E10" t="b">
+        <v>1</v>
+      </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A11">
@@ -2200,6 +2227,9 @@
       <c r="D11">
         <v>485</v>
       </c>
+      <c r="E11" t="b">
+        <v>1</v>
+      </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A12">
@@ -2214,6 +2244,9 @@
       <c r="D12">
         <v>322</v>
       </c>
+      <c r="E12" t="b">
+        <v>1</v>
+      </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A13">
@@ -2228,6 +2261,9 @@
       <c r="D13">
         <v>51</v>
       </c>
+      <c r="E13" t="b">
+        <v>1</v>
+      </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A14">
@@ -2242,6 +2278,9 @@
       <c r="D14">
         <v>152</v>
       </c>
+      <c r="E14" t="b">
+        <v>1</v>
+      </c>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A15">
@@ -2256,6 +2295,9 @@
       <c r="D15">
         <v>634</v>
       </c>
+      <c r="E15" t="b">
+        <v>1</v>
+      </c>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A16">
@@ -2270,8 +2312,11 @@
       <c r="D16">
         <v>299</v>
       </c>
-    </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E16" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A17">
         <v>10001606</v>
       </c>
@@ -2284,8 +2329,11 @@
       <c r="D17">
         <v>466</v>
       </c>
-    </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E17" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A18">
         <v>10001622</v>
       </c>
@@ -2298,8 +2346,11 @@
       <c r="D18">
         <v>971</v>
       </c>
-    </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E18" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A19">
         <v>10001772</v>
       </c>
@@ -2312,8 +2363,11 @@
       <c r="D19">
         <v>434</v>
       </c>
-    </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E19" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A20">
         <v>10001979</v>
       </c>
@@ -2326,8 +2380,11 @@
       <c r="D20">
         <v>228</v>
       </c>
-    </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E20" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A21">
         <v>10001998</v>
       </c>
@@ -2340,8 +2397,11 @@
       <c r="D21">
         <v>142</v>
       </c>
-    </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E21" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A22">
         <v>10002012</v>
       </c>
@@ -2354,8 +2414,11 @@
       <c r="D22">
         <v>789</v>
       </c>
-    </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E22" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A23">
         <v>10002310</v>
       </c>
@@ -2368,8 +2431,11 @@
       <c r="D23">
         <v>924</v>
       </c>
-    </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E23" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A24">
         <v>10002475</v>
       </c>
@@ -2382,8 +2448,11 @@
       <c r="D24">
         <v>206</v>
       </c>
-    </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E24" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A25">
         <v>10002563</v>
       </c>
@@ -2396,8 +2465,11 @@
       <c r="D25">
         <v>832</v>
       </c>
-    </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E25" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A26">
         <v>10002647</v>
       </c>
@@ -2410,8 +2482,11 @@
       <c r="D26">
         <v>712</v>
       </c>
-    </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E26" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A27">
         <v>10002713</v>
       </c>
@@ -2424,8 +2499,11 @@
       <c r="D27">
         <v>781</v>
       </c>
-    </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E27" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A28">
         <v>10002885</v>
       </c>
@@ -2438,8 +2516,11 @@
       <c r="D28">
         <v>977</v>
       </c>
-    </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E28" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A29">
         <v>10002968</v>
       </c>
@@ -2452,8 +2533,11 @@
       <c r="D29">
         <v>95</v>
       </c>
-    </row>
-    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E29" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="30" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A30">
         <v>10003012</v>
       </c>
@@ -2466,8 +2550,11 @@
       <c r="D30">
         <v>315</v>
       </c>
-    </row>
-    <row r="31" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E30" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="31" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A31">
         <v>10003061</v>
       </c>
@@ -2480,8 +2567,11 @@
       <c r="D31">
         <v>433</v>
       </c>
-    </row>
-    <row r="32" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E31" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="32" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A32">
         <v>10003072</v>
       </c>
@@ -2494,8 +2584,11 @@
       <c r="D32">
         <v>495</v>
       </c>
-    </row>
-    <row r="33" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E32" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="33" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A33">
         <v>10003623</v>
       </c>
@@ -2508,8 +2601,11 @@
       <c r="D33">
         <v>24</v>
       </c>
-    </row>
-    <row r="34" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E33" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="34" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A34">
         <v>10003715</v>
       </c>
@@ -2522,8 +2618,11 @@
       <c r="D34">
         <v>263</v>
       </c>
-    </row>
-    <row r="35" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E34" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="35" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A35">
         <v>10003833</v>
       </c>
@@ -2536,8 +2635,11 @@
       <c r="D35">
         <v>810</v>
       </c>
-    </row>
-    <row r="36" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E35" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="36" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A36">
         <v>10003846</v>
       </c>
@@ -2550,8 +2652,11 @@
       <c r="D36">
         <v>637</v>
       </c>
-    </row>
-    <row r="37" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E36" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="37" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A37">
         <v>10004015</v>
       </c>
@@ -2564,8 +2669,11 @@
       <c r="D37">
         <v>804</v>
       </c>
-    </row>
-    <row r="38" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E37" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="38" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A38">
         <v>10004086</v>
       </c>
@@ -2578,8 +2686,11 @@
       <c r="D38">
         <v>933</v>
       </c>
-    </row>
-    <row r="39" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E38" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="39" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A39">
         <v>10004495</v>
       </c>
@@ -2592,8 +2703,11 @@
       <c r="D39">
         <v>595</v>
       </c>
-    </row>
-    <row r="40" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E39" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="40" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A40">
         <v>10004667</v>
       </c>
@@ -2605,6 +2719,9 @@
       </c>
       <c r="D40">
         <v>557</v>
+      </c>
+      <c r="E40" t="b">
+        <v>1</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Finished writing Order Details sequence
</commit_message>
<xml_diff>
--- a/CMPG323 EcoPower Logistics Data.xlsx
+++ b/CMPG323 EcoPower Logistics Data.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\1_3rd_year_uni\CMPG323\CMPG323_Project4\CMPG-323-Project-4-40604012\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3F87F251-6633-489A-AC09-5E2696DD8E89}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FEBC481B-2429-4208-9C17-5F2FD162627B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-18180" yWindow="-525" windowWidth="15375" windowHeight="7875" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-18180" yWindow="-525" windowWidth="15375" windowHeight="7875" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Customers" sheetId="1" r:id="rId1"/>
@@ -1032,7 +1032,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:F41"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A32" workbookViewId="0">
       <selection activeCell="F1" sqref="F1"/>
     </sheetView>
   </sheetViews>
@@ -1081,6 +1081,9 @@
       <c r="E2">
         <v>0</v>
       </c>
+      <c r="F2" t="b">
+        <v>1</v>
+      </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3">
@@ -1098,6 +1101,9 @@
       <c r="E3">
         <v>0</v>
       </c>
+      <c r="F3" t="b">
+        <v>1</v>
+      </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4">
@@ -1115,6 +1121,9 @@
       <c r="E4">
         <v>0</v>
       </c>
+      <c r="F4" t="b">
+        <v>1</v>
+      </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5">
@@ -1132,6 +1141,9 @@
       <c r="E5">
         <v>0</v>
       </c>
+      <c r="F5" t="b">
+        <v>1</v>
+      </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6">
@@ -1149,6 +1161,9 @@
       <c r="E6">
         <v>0.7</v>
       </c>
+      <c r="F6" t="b">
+        <v>1</v>
+      </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7">
@@ -1166,6 +1181,9 @@
       <c r="E7">
         <v>0.2</v>
       </c>
+      <c r="F7" t="b">
+        <v>1</v>
+      </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8">
@@ -1183,6 +1201,9 @@
       <c r="E8">
         <v>0.2</v>
       </c>
+      <c r="F8" t="b">
+        <v>1</v>
+      </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A9">
@@ -1200,6 +1221,9 @@
       <c r="E9">
         <v>0.2</v>
       </c>
+      <c r="F9" t="b">
+        <v>1</v>
+      </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A10">
@@ -1217,6 +1241,9 @@
       <c r="E10">
         <v>0.2</v>
       </c>
+      <c r="F10" t="b">
+        <v>1</v>
+      </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A11">
@@ -1234,6 +1261,9 @@
       <c r="E11">
         <v>0.2</v>
       </c>
+      <c r="F11" t="b">
+        <v>1</v>
+      </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A12">
@@ -1251,6 +1281,9 @@
       <c r="E12">
         <v>0.2</v>
       </c>
+      <c r="F12" t="b">
+        <v>1</v>
+      </c>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A13">
@@ -1268,6 +1301,9 @@
       <c r="E13">
         <v>0.2</v>
       </c>
+      <c r="F13" t="b">
+        <v>1</v>
+      </c>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A14">
@@ -1285,6 +1321,9 @@
       <c r="E14">
         <v>0</v>
       </c>
+      <c r="F14" t="b">
+        <v>1</v>
+      </c>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A15">
@@ -1302,6 +1341,9 @@
       <c r="E15">
         <v>0</v>
       </c>
+      <c r="F15" t="b">
+        <v>1</v>
+      </c>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A16">
@@ -1319,8 +1361,11 @@
       <c r="E16">
         <v>0</v>
       </c>
-    </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F16" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A17">
         <v>6091</v>
       </c>
@@ -1336,8 +1381,11 @@
       <c r="E17">
         <v>0.1</v>
       </c>
-    </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F17" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A18">
         <v>6092</v>
       </c>
@@ -1353,8 +1401,11 @@
       <c r="E18">
         <v>0</v>
       </c>
-    </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F18" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A19">
         <v>6093</v>
       </c>
@@ -1370,8 +1421,11 @@
       <c r="E19">
         <v>0</v>
       </c>
-    </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F19" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A20">
         <v>6094</v>
       </c>
@@ -1387,8 +1441,11 @@
       <c r="E20">
         <v>0</v>
       </c>
-    </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F20" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A21">
         <v>6095</v>
       </c>
@@ -1404,8 +1461,11 @@
       <c r="E21">
         <v>0</v>
       </c>
-    </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F21" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A22">
         <v>6096</v>
       </c>
@@ -1421,8 +1481,11 @@
       <c r="E22">
         <v>0</v>
       </c>
-    </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F22" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A23">
         <v>6097</v>
       </c>
@@ -1438,8 +1501,11 @@
       <c r="E23">
         <v>0.1</v>
       </c>
-    </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F23" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A24">
         <v>6098</v>
       </c>
@@ -1455,8 +1521,11 @@
       <c r="E24">
         <v>0.2</v>
       </c>
-    </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F24" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A25">
         <v>6099</v>
       </c>
@@ -1472,8 +1541,11 @@
       <c r="E25">
         <v>0</v>
       </c>
-    </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F25" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="26" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A26">
         <v>6100</v>
       </c>
@@ -1489,8 +1561,11 @@
       <c r="E26">
         <v>0.1</v>
       </c>
-    </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F26" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="27" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A27">
         <v>6101</v>
       </c>
@@ -1506,8 +1581,11 @@
       <c r="E27">
         <v>0</v>
       </c>
-    </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F27" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="28" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A28">
         <v>6102</v>
       </c>
@@ -1523,8 +1601,11 @@
       <c r="E28">
         <v>0.1</v>
       </c>
-    </row>
-    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F28" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="29" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A29">
         <v>6103</v>
       </c>
@@ -1540,8 +1621,11 @@
       <c r="E29">
         <v>0</v>
       </c>
-    </row>
-    <row r="30" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F29" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="30" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A30">
         <v>6104</v>
       </c>
@@ -1557,8 +1641,11 @@
       <c r="E30">
         <v>0</v>
       </c>
-    </row>
-    <row r="31" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F30" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="31" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A31">
         <v>6288</v>
       </c>
@@ -1574,8 +1661,11 @@
       <c r="E31">
         <v>0.2</v>
       </c>
-    </row>
-    <row r="32" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F31" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="32" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A32">
         <v>6289</v>
       </c>
@@ -1591,8 +1681,11 @@
       <c r="E32">
         <v>0.2</v>
       </c>
-    </row>
-    <row r="33" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F32" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="33" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A33">
         <v>7320</v>
       </c>
@@ -1608,8 +1701,11 @@
       <c r="E33">
         <v>0</v>
       </c>
-    </row>
-    <row r="34" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F33" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="34" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A34">
         <v>7321</v>
       </c>
@@ -1625,8 +1721,11 @@
       <c r="E34">
         <v>0</v>
       </c>
-    </row>
-    <row r="35" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F34" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="35" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A35">
         <v>7404</v>
       </c>
@@ -1642,8 +1741,11 @@
       <c r="E35">
         <v>0.15</v>
       </c>
-    </row>
-    <row r="36" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F35" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="36" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A36">
         <v>7405</v>
       </c>
@@ -1659,8 +1761,11 @@
       <c r="E36">
         <v>0</v>
       </c>
-    </row>
-    <row r="37" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F36" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="37" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A37">
         <v>7406</v>
       </c>
@@ -1676,8 +1781,11 @@
       <c r="E37">
         <v>0.2</v>
       </c>
-    </row>
-    <row r="38" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F37" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="38" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A38">
         <v>7407</v>
       </c>
@@ -1693,8 +1801,11 @@
       <c r="E38">
         <v>0.2</v>
       </c>
-    </row>
-    <row r="39" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F38" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="39" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A39">
         <v>9132</v>
       </c>
@@ -1710,8 +1821,11 @@
       <c r="E39">
         <v>0</v>
       </c>
-    </row>
-    <row r="40" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F39" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="40" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A40">
         <v>9133</v>
       </c>
@@ -1727,8 +1841,11 @@
       <c r="E40">
         <v>0</v>
       </c>
-    </row>
-    <row r="41" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F40" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="41" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A41">
         <v>9737</v>
       </c>
@@ -1743,6 +1860,9 @@
       </c>
       <c r="E41">
         <v>0</v>
+      </c>
+      <c r="F41" t="b">
+        <v>1</v>
       </c>
     </row>
   </sheetData>
@@ -2031,7 +2151,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:E40"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A31" workbookViewId="0">
+    <sheetView topLeftCell="A31" workbookViewId="0">
       <selection activeCell="E1" sqref="E1"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Added all workflows to main with options to choose which object to test
</commit_message>
<xml_diff>
--- a/CMPG323 EcoPower Logistics Data.xlsx
+++ b/CMPG323 EcoPower Logistics Data.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\1_3rd_year_uni\CMPG323\CMPG323_Project4\CMPG-323-Project-4-40604012\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FEBC481B-2429-4208-9C17-5F2FD162627B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{541B30F1-E3DB-4FDE-B021-6FDB2A94C41D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-18180" yWindow="-525" windowWidth="15375" windowHeight="7875" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="2130" yWindow="1365" windowWidth="15375" windowHeight="7875" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Customers" sheetId="1" r:id="rId1"/>
@@ -732,8 +732,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:F14"/>
   <sheetViews>
-    <sheetView topLeftCell="A11" workbookViewId="0">
-      <selection activeCell="G2" sqref="G2"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F2" sqref="F2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1032,7 +1032,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:F41"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A32" workbookViewId="0">
+    <sheetView topLeftCell="A32" workbookViewId="0">
       <selection activeCell="F1" sqref="F1"/>
     </sheetView>
   </sheetViews>
@@ -1874,8 +1874,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:E15"/>
   <sheetViews>
-    <sheetView topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="E2" sqref="E2"/>
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="E1" sqref="E1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
Begun adding logout functionality
</commit_message>
<xml_diff>
--- a/CMPG323 EcoPower Logistics Data.xlsx
+++ b/CMPG323 EcoPower Logistics Data.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\1_3rd_year_uni\CMPG323\CMPG323_Project4\CMPG-323-Project-4-40604012\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{541B30F1-E3DB-4FDE-B021-6FDB2A94C41D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C870D776-CC5C-48CB-8BFA-958C05F529B4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2130" yWindow="1365" windowWidth="15375" windowHeight="7875" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="2130" yWindow="1365" windowWidth="15375" windowHeight="7875" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Customers" sheetId="1" r:id="rId1"/>
@@ -732,7 +732,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:F14"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView topLeftCell="A7" workbookViewId="0">
       <selection activeCell="F2" sqref="F2"/>
     </sheetView>
   </sheetViews>
@@ -1032,8 +1032,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:F41"/>
   <sheetViews>
-    <sheetView topLeftCell="A32" workbookViewId="0">
-      <selection activeCell="F1" sqref="F1"/>
+    <sheetView tabSelected="1" topLeftCell="A28" workbookViewId="0">
+      <selection activeCell="F2" sqref="F2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1874,8 +1874,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:E15"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="E1" sqref="E1"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E2" sqref="E2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2152,7 +2152,7 @@
   <dimension ref="A1:E40"/>
   <sheetViews>
     <sheetView topLeftCell="A31" workbookViewId="0">
-      <selection activeCell="E1" sqref="E1"/>
+      <selection activeCell="E2" sqref="E2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
Fixed an error in the workflow order
</commit_message>
<xml_diff>
--- a/CMPG323 EcoPower Logistics Data.xlsx
+++ b/CMPG323 EcoPower Logistics Data.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\1_3rd_year_uni\CMPG323\CMPG323_Project4\CMPG-323-Project-4-40604012\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C870D776-CC5C-48CB-8BFA-958C05F529B4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9FADB6CD-5B3E-4961-A2E6-035620188CB9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2130" yWindow="1365" windowWidth="15375" windowHeight="7875" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="2130" yWindow="1365" windowWidth="15375" windowHeight="7875" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Customers" sheetId="1" r:id="rId1"/>
@@ -732,7 +732,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:F14"/>
   <sheetViews>
-    <sheetView topLeftCell="A7" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
       <selection activeCell="F2" sqref="F2"/>
     </sheetView>
   </sheetViews>
@@ -1032,7 +1032,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:F41"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A28" workbookViewId="0">
+    <sheetView topLeftCell="A28" workbookViewId="0">
       <selection activeCell="F2" sqref="F2"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Fixed problem of getting an error when there are multiple rows - Customers
</commit_message>
<xml_diff>
--- a/CMPG323 EcoPower Logistics Data.xlsx
+++ b/CMPG323 EcoPower Logistics Data.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\1_3rd_year_uni\CMPG323\CMPG323_Project4\CMPG-323-Project-4-40604012\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9FADB6CD-5B3E-4961-A2E6-035620188CB9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{365B3509-ECC9-48A3-97D7-B7DF98CD5DFA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="2130" yWindow="1365" windowWidth="15375" windowHeight="7875" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1875,7 +1875,7 @@
   <dimension ref="A1:E15"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E2" sqref="E2"/>
+      <selection activeCell="E3" sqref="E3:E4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2297,7 +2297,7 @@
         <v>709</v>
       </c>
       <c r="E8" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Fixed problem of getting an error when there are multiple rows - Orders
</commit_message>
<xml_diff>
--- a/CMPG323 EcoPower Logistics Data.xlsx
+++ b/CMPG323 EcoPower Logistics Data.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\1_3rd_year_uni\CMPG323\CMPG323_Project4\CMPG-323-Project-4-40604012\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{365B3509-ECC9-48A3-97D7-B7DF98CD5DFA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BA31C640-0F0F-4A7E-A0E6-D402CE2DE8F6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2130" yWindow="1365" windowWidth="15375" windowHeight="7875" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="2130" yWindow="1365" windowWidth="15375" windowHeight="7875" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Customers" sheetId="1" r:id="rId1"/>
@@ -732,7 +732,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:F14"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+    <sheetView topLeftCell="A7" workbookViewId="0">
       <selection activeCell="F2" sqref="F2"/>
     </sheetView>
   </sheetViews>
@@ -1874,7 +1874,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:E15"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="E3" sqref="E3:E4"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Fixed problem of getting an error when there are multiple rows - Products
</commit_message>
<xml_diff>
--- a/CMPG323 EcoPower Logistics Data.xlsx
+++ b/CMPG323 EcoPower Logistics Data.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\1_3rd_year_uni\CMPG323\CMPG323_Project4\CMPG-323-Project-4-40604012\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BA31C640-0F0F-4A7E-A0E6-D402CE2DE8F6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E5CE610B-7427-4814-9876-8B470549D324}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2130" yWindow="1365" windowWidth="15375" windowHeight="7875" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="2130" yWindow="1365" windowWidth="15375" windowHeight="7875" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Customers" sheetId="1" r:id="rId1"/>
@@ -1032,7 +1032,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:F41"/>
   <sheetViews>
-    <sheetView topLeftCell="A28" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A28" workbookViewId="0">
       <selection activeCell="F2" sqref="F2"/>
     </sheetView>
   </sheetViews>
@@ -1874,7 +1874,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:E15"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="E3" sqref="E3:E4"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Did final testing and deleted un-needed test sequence
</commit_message>
<xml_diff>
--- a/CMPG323 EcoPower Logistics Data.xlsx
+++ b/CMPG323 EcoPower Logistics Data.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\1_3rd_year_uni\CMPG323\CMPG323_Project4\CMPG-323-Project-4-40604012\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E5CE610B-7427-4814-9876-8B470549D324}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{220E2FD6-D173-4F30-8A1E-CE4F9B486D9B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2130" yWindow="1365" windowWidth="15375" windowHeight="7875" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-18930" yWindow="525" windowWidth="15375" windowHeight="7875" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Customers" sheetId="1" r:id="rId1"/>
@@ -1032,8 +1032,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:F41"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A28" workbookViewId="0">
-      <selection activeCell="F2" sqref="F2"/>
+    <sheetView tabSelected="1" topLeftCell="A34" workbookViewId="0">
+      <selection activeCell="F2" sqref="F2:F41"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1874,8 +1874,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:E15"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E3" sqref="E3:E4"/>
+    <sheetView topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="E15" sqref="E15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2151,7 +2151,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:E40"/>
   <sheetViews>
-    <sheetView topLeftCell="A31" workbookViewId="0">
+    <sheetView topLeftCell="A40" workbookViewId="0">
       <selection activeCell="E2" sqref="E2"/>
     </sheetView>
   </sheetViews>
@@ -2297,7 +2297,7 @@
         <v>709</v>
       </c>
       <c r="E8" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.25">

</xml_diff>